<commit_message>
Tube formation model added Extra analysis added to include the model for the pollen tube formation
</commit_message>
<xml_diff>
--- a/PollenDeposition/data_deposition.xlsx
+++ b/PollenDeposition/data_deposition.xlsx
@@ -12686,7 +12686,12 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="affc661c-8544-473e-8a75-53d960e38a08">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="22626614-c5d1-4627-a764-7e7b201e97f2" xsi:nil="true"/>
+  </documentManagement>
 </p:properties>
 </file>
 
@@ -12700,9 +12705,10 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002031DAFB2DC2FB44B6DE2DC8257168D2" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="da7341311a534ad4a8459efdf2e60f2c">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2c798e8e-9291-4c6e-a57a-485864a2de66" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7fc1bfb0dcaba3a80823fa931d57aebf" ns2:_="">
-    <xsd:import namespace="2c798e8e-9291-4c6e-a57a-485864a2de66"/>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100BA1DD7ED721C9F4885394B10D48B4E67" ma:contentTypeVersion="16" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="ea15fde66788084ea503513845884e5f">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="affc661c-8544-473e-8a75-53d960e38a08" xmlns:ns3="22626614-c5d1-4627-a764-7e7b201e97f2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0cd04f0dc3d2a27992778f2373fc6e4b" ns2:_="" ns3:_="">
+    <xsd:import namespace="affc661c-8544-473e-8a75-53d960e38a08"/>
+    <xsd:import namespace="22626614-c5d1-4627-a764-7e7b201e97f2"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -12713,6 +12719,17 @@
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -12720,7 +12737,7 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="2c798e8e-9291-4c6e-a57a-485864a2de66" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="affc661c-8544-473e-8a75-53d960e38a08" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
@@ -12745,6 +12762,91 @@
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="14" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="15" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="16" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="17" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="18" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="20" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="22" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Bildemerkelapper" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="34b671a8-374e-43c3-b91a-c5799fa485d4" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="22626614-c5d1-4627-a764-7e7b201e97f2" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="12" nillable="true" ma:displayName="Delt med" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="13" nillable="true" ma:displayName="Delingsdetaljer" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="23" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{e52b70dc-723d-43f6-b79d-9bf9a083b723}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="22626614-c5d1-4627-a764-7e7b201e97f2">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
     <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
@@ -12755,8 +12857,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Innholdstype"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Tittel"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -12854,5 +12956,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CAA40D3-A772-4411-B2FF-91CEE34E52B5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A5376AC-EBFF-42F9-B3EF-1F672DA4E823}"/>
 </file>
</xml_diff>